<commit_message>
Add generation of graphs Set back only one producer
</commit_message>
<xml_diff>
--- a/DiagramUML.xlsx
+++ b/DiagramUML.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pro\Git\RepartKey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{908EFFA6-1CA7-4A5B-8236-9FA569649852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0EDCA2-5B62-4EAB-9742-9775192116FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{665AF352-CB8A-4CDE-86A3-C43EB7FF9127}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C2CFD62-ECDA-47A9-B5F1-6188C6239BA5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="StateMachine" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,10 +25,107 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>prm</t>
+  </si>
+  <si>
+    <t>point_list</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>Repartition</t>
+  </si>
+  <si>
+    <t>point_list[nb_slot]</t>
+  </si>
+  <si>
+    <t>priority_list[nb_prod]</t>
+  </si>
+  <si>
+    <t>ratio_list[nb_prod]</t>
+  </si>
+  <si>
+    <t>prm_list</t>
+  </si>
+  <si>
+    <t>ConsRepart</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>auto_consumption</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>ProdRepart</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>Param</t>
+  </si>
+  <si>
+    <t>prod_list[nb_prod]</t>
+  </si>
+  <si>
+    <t>cons_list[nb_cons]</t>
+  </si>
+  <si>
+    <t>param_list[nb_prod]</t>
+  </si>
+  <si>
+    <t>initial_production</t>
+  </si>
+  <si>
+    <t>prod_to_remove</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -43,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -51,12 +149,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,6 +226,517 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit avec flèche 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57EC9052-68E2-EF25-50EF-FDF6948BA761}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2362200" y="1552575"/>
+          <a:ext cx="9525" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>558362</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>558362</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABCCA00B-353F-48EF-850A-FE0B7F36EB13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4197569" y="1149569"/>
+          <a:ext cx="0" cy="939362"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle : coins arrondis 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EDF1DC5-0BE9-E74F-5888-698BA5467F9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076326" y="285750"/>
+          <a:ext cx="2095500" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle : coins arrondis 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E27E5CA1-87F3-40D7-906E-8FD3C1D9AE34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3381375" y="266700"/>
+          <a:ext cx="1600200" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>577741</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14123</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>587500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E6E743-2017-4AAA-A981-0FBC73221374}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8256862" y="966623"/>
+          <a:ext cx="9759" cy="1122308"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>624052</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connecteur droit avec flèche 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{086E3196-B4A9-4EAC-ADF7-7735A9E60CB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7015655" y="2590800"/>
+          <a:ext cx="672991" cy="673976"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle : coins arrondis 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5BEE323-67F0-41C9-A351-FF9355F9DDFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6181725" y="238123"/>
+          <a:ext cx="4143375" cy="5143502"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 8429"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>98534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connecteur droit avec flèche 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05E19EEB-83D4-4702-9796-8B0EEE40F652}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8874672" y="2765534"/>
+          <a:ext cx="412531" cy="472966"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>643759</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connecteur droit avec flèche 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B3F6E0-4D1B-46E0-ADA0-DD6BB89788AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7035362" y="4013638"/>
+          <a:ext cx="3941" cy="367862"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +1035,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FDB9E5-C1BD-4527-8C89-FA10B435171E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F2D3C-16EC-4CC9-A743-33A78D062162}">
+  <dimension ref="C3:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67619396-70A3-4137-AA10-7F774515C666}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add additional methods to compute statistics Add simulation files for Antony Soleil
</commit_message>
<xml_diff>
--- a/DiagramUML.xlsx
+++ b/DiagramUML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pro\Git\RepartKey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0EDCA2-5B62-4EAB-9742-9775192116FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A73BEB-E4F2-43C2-A792-4767099A2669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C2CFD62-ECDA-47A9-B5F1-6188C6239BA5}"/>
   </bookViews>
@@ -339,7 +339,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>490904</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
@@ -362,8 +362,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1076326" y="285750"/>
-          <a:ext cx="2095500" cy="2781300"/>
+          <a:off x="1252904" y="285750"/>
+          <a:ext cx="1921853" cy="2781300"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -465,13 +465,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>577741</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>14123</xdr:rowOff>
+      <xdr:rowOff>6796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>587500</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>183931</xdr:rowOff>
+      <xdr:colOff>577741</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -486,8 +486,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8256862" y="966623"/>
-          <a:ext cx="9759" cy="1122308"/>
+          <a:off x="8263683" y="959296"/>
+          <a:ext cx="0" cy="366877"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -516,15 +516,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>624052</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>644769</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>26276</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1282211</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -539,8 +539,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7015655" y="2590800"/>
-          <a:ext cx="672991" cy="673976"/>
+          <a:off x="7041173" y="1846385"/>
+          <a:ext cx="637442" cy="622788"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -569,15 +569,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>631581</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47623</xdr:rowOff>
+      <xdr:rowOff>40296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>183173</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -592,8 +592,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6181725" y="238123"/>
-          <a:ext cx="4143375" cy="5143502"/>
+          <a:off x="6207369" y="230796"/>
+          <a:ext cx="3991708" cy="4311896"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -634,13 +634,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>6569</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>98534</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -687,13 +687,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>643759</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>13138</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1036,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F2D3C-16EC-4CC9-A743-33A78D062162}">
-  <dimension ref="C3:J27"/>
+  <dimension ref="C3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,7 @@
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1093,103 +1093,105 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I15" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="2" t="s">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>20</v>
+      <c r="H20" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H26" s="3" t="s">
+    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H27" s="4" t="s">
+    <row r="23" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1203,7 +1205,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67619396-70A3-4137-AA10-7F774515C666}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add function to compute dynamic keys
</commit_message>
<xml_diff>
--- a/DiagramUML.xlsx
+++ b/DiagramUML.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pro\Git\RepartKey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A73BEB-E4F2-43C2-A792-4767099A2669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2007E1C-879C-4C73-89DC-74D2B114DEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C2CFD62-ECDA-47A9-B5F1-6188C6239BA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9C2CFD62-ECDA-47A9-B5F1-6188C6239BA5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="UML Diagram" sheetId="1" r:id="rId1"/>
     <sheet name="StateMachine" sheetId="2" r:id="rId2"/>
+    <sheet name="Dynamic key" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Consumer</t>
   </si>
@@ -110,12 +111,51 @@
   </si>
   <si>
     <t>state</t>
+  </si>
+  <si>
+    <t>Consommateur</t>
+  </si>
+  <si>
+    <t>Consommation</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Producteur</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Ratio conso/prod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,12 +245,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95F2D3C-16EC-4CC9-A743-33A78D062162}">
   <dimension ref="C3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1213,4 +1259,203 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D160B451-286F-4F4E-B3AD-636D956B12B6}">
+  <dimension ref="B3:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <f>C4/C$7</f>
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="6">
+        <f>$D4*$C$10*$C$14</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="I4" s="6">
+        <f>$D4*$C$11*$C$14</f>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(H4:I4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D6" si="0">C5/C$7</f>
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" ref="H5:H6" si="1">$D5*$C$10*$C$14</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" ref="I5:I6" si="2">$D5*$C$11*$C$14</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J6" si="3">SUM(H5:I5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K6" s="7">
+        <f>SUM(J4:J6)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5">
+        <f>SUM(C4:C6)</f>
+        <v>10</v>
+      </c>
+      <c r="H7" s="7">
+        <f>SUM(H4:H6)</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="I7" s="7">
+        <f>SUM(I4:I6)</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="7">
+        <f>SUM(H7:I7)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8">
+        <f>C10/C$12</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8">
+        <f>C11/C$12</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5">
+        <f>SUM(C10:C11)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="10">
+        <f>IF(C7&gt;C12,1,C7/C12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>